<commit_message>
Auto-committed on 2023/09/27 週三 11:55:57.05
</commit_message>
<xml_diff>
--- a/Program/Other/LP006_底稿_房貸協辦人員異動名單.xlsx
+++ b/Program/Other/LP006_底稿_房貸協辦人員異動名單.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\itxWrite\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SKL_SVN\iTX\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF15D2F8-D878-4ED0-9AFB-2EDB2733E32A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB2BECD-50BD-444B-B903-A5F3A1FB3A1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="791" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="791" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="異動名單" sheetId="70" r:id="rId1"/>
@@ -94,10 +94,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>考核前職級</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>異動原因</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -111,6 +107,10 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>考核後職級</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -121,7 +121,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <name val="新細明體"/>
@@ -146,6 +146,12 @@
       <sz val="12"/>
       <name val="標楷體"/>
       <family val="4"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="新細明體"/>
+      <family val="1"/>
       <charset val="136"/>
     </font>
   </fonts>
@@ -181,7 +187,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -191,8 +197,9 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -208,10 +215,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
     <cellStyle name="一般 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="一般_9804" xfId="3" xr:uid="{9770F826-B890-4CE9-AC67-F1E71CB600CE}"/>
     <cellStyle name="千分位 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -603,7 +614,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.6640625" defaultRowHeight="16.2"/>
@@ -621,7 +632,7 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -654,16 +665,16 @@
       <c r="G2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -676,31 +687,31 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>